<commit_message>
Ajout dictionnaire des mots
</commit_message>
<xml_diff>
--- a/pythonFile/stopwords-fr.xlsx
+++ b/pythonFile/stopwords-fr.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\François\Documents\Cours 2022-2023\PPD\LobsterTwitterScrapping\pythonFile\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FTG1\Documents\Projects\Lobster\LobsterTwitterScrapping\pythonFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE582121-9B33-48B3-A274-5972B85A857B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E1DC4F7B-C609-4D21-A2B7-F472474DF032}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$A$1</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="752">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="755">
   <si>
     <t>a</t>
   </si>
@@ -2293,12 +2292,21 @@
   </si>
   <si>
     <t>vs</t>
+  </si>
+  <si>
+    <t>https</t>
+  </si>
+  <si>
+    <t>of</t>
+  </si>
+  <si>
+    <t>é</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2643,14 +2651,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C90387F1-53C8-42D4-B4CC-3528475A95F2}">
-  <dimension ref="A1:A786"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A789"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A720" workbookViewId="0">
-      <selection activeCell="E739" sqref="E739"/>
+    <sheetView tabSelected="1" topLeftCell="A777" workbookViewId="0">
+      <selection activeCell="A790" sqref="A790"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -6577,8 +6585,23 @@
         <v>102</v>
       </c>
     </row>
+    <row r="787" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A787" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="788" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A788" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="789" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A789" t="s">
+        <v>754</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1" xr:uid="{C90387F1-53C8-42D4-B4CC-3528475A95F2}"/>
+  <autoFilter ref="A1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>